<commit_message>
Adjust difficult ramp for Expert
</commit_message>
<xml_diff>
--- a/HigherDifficulty/Higher Difficulty mod.xlsx
+++ b/HigherDifficulty/Higher Difficulty mod.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Git\BepInEx Modding\Void Crew\HigherDifficulty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6B42CCE-69DF-4C6A-9FBF-7850F4BD0008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8497FF40-C3D0-4566-8E0B-3B5EBC434A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{3E5625EC-FE87-4A90-9D77-E9CEC83E5F9C}"/>
+    <workbookView xWindow="14317" yWindow="0" windowWidth="14565" windowHeight="15563" xr2:uid="{3E5625EC-FE87-4A90-9D77-E9CEC83E5F9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Higher Difficulty mod" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,14 @@
       <sz val="9.8000000000000007"/>
       <name val="Iosevka"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -124,11 +132,190 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.8000000000000007"/>
+        <color auto="1"/>
+        <name val="Iosevka"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.8000000000000007"/>
+        <color auto="1"/>
+        <name val="Iosevka"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.8000000000000007"/>
+        <color auto="1"/>
+        <name val="Iosevka"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.8000000000000007"/>
+        <color auto="1"/>
+        <name val="Iosevka"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.8000000000000007"/>
+        <color auto="1"/>
+        <name val="Iosevka"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -139,6 +326,54 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{66FF5D76-FE39-4CFE-8EFD-142C9DB7D0D4}" name="Normal" displayName="Normal" ref="A1:C6">
+  <autoFilter ref="A1:C6" xr:uid="{66FF5D76-FE39-4CFE-8EFD-142C9DB7D0D4}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{ED02291A-3D5C-41CA-85CB-961B4D193482}" name="Normal Difficulty" totalsRowLabel="Total" dataDxfId="16" totalsRowDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{0D6627B3-EC59-481C-AA98-483579AB0F91}" name="Old" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{904A8C84-5C89-4BEE-B1AF-0034C88EF15E}" name="New" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9885C985-0606-4ED4-8426-9693631BB2EA}" name="Veteran" displayName="Veteran" ref="A8:C13" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A8:C13" xr:uid="{9885C985-0606-4ED4-8426-9693631BB2EA}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{0D923107-BF92-4A9A-86C6-0C6BA84EFF13}" name="Veteran Difficulty" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{83139A98-6E6C-4CF3-9E4D-B56AC5DF7F9D}" name="Old" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{73979D49-EAF9-402E-AC76-C52DAF829E71}" name="New" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C2B2EF74-7025-48D8-B0FA-D9302D716664}" name="Expert" displayName="Expert" ref="A15:C20" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A15:C20" xr:uid="{C2B2EF74-7025-48D8-B0FA-D9302D716664}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{CD882121-43AA-439F-BB53-AACAA28C453E}" name="Expert Difficulty" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{CBE7C3DE-8598-49AF-B08E-80DD8911C0AA}" name="Old" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{6BA31C39-A104-4DBB-B792-A8D0637882B4}" name="New" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A57C28CC-1E21-434D-A4FC-219451F5CC8B}" name="Insane" displayName="Insane" ref="A22:C27" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A22:C27" xr:uid="{A57C28CC-1E21-434D-A4FC-219451F5CC8B}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{15757A4D-B241-466F-921C-9CF0A6BF3D3E}" name="Insane Difficulty" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{925B2AD5-0E54-43D1-B3CE-BEC6F94D813B}" name="Old" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{CB4FCAEB-24CE-4802-A375-9C9A261538EC}" name="New" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,7 +675,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3324A5EA-CC3F-4480-AE96-A50260F385F3}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -519,13 +756,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -548,7 +785,7 @@
         <v>-0.25</v>
       </c>
       <c r="C10" s="2">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
@@ -559,7 +796,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="2">
-        <v>1</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
@@ -572,7 +809,7 @@
       </c>
       <c r="C12" s="2">
         <f>(1+C9)*(1+C10)*(1+C11)</f>
-        <v>2.6449999999999996</v>
+        <v>2.254</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
@@ -581,17 +818,17 @@
       </c>
       <c r="C13" s="2">
         <f>C12/B12</f>
-        <v>4.7022222222222219</v>
+        <v>4.0071111111111115</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+      <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -603,7 +840,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="2">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
@@ -614,7 +851,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="2">
-        <v>0.32500000000000001</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
@@ -625,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="2">
-        <v>2.25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
@@ -638,7 +875,7 @@
       </c>
       <c r="C19" s="2">
         <f>(1+C16)*(1+C17)*(1+C18)</f>
-        <v>5.3828125</v>
+        <v>4.0200000000000005</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
@@ -647,17 +884,17 @@
       </c>
       <c r="C20" s="2">
         <f>C19/B19</f>
-        <v>5.3828125</v>
+        <v>4.0200000000000005</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+      <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B22" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -666,10 +903,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="2">
-        <v>-0.25</v>
-      </c>
-      <c r="C23" s="2">
         <v>0.25</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
@@ -677,7 +914,7 @@
         <v>3</v>
       </c>
       <c r="B24" s="2">
-        <v>-0.25</v>
+        <v>0.25</v>
       </c>
       <c r="C24" s="2">
         <v>0.5</v>
@@ -700,11 +937,11 @@
       </c>
       <c r="B26" s="2">
         <f>(1+B23)*(1+B24)*(1+B25)</f>
-        <v>0.5625</v>
+        <v>1.5625</v>
       </c>
       <c r="C26" s="2">
         <f>(1+C23)*(1+C24)*(1+C25)</f>
-        <v>6.09375</v>
+        <v>6.3375000000000004</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
@@ -713,11 +950,17 @@
       </c>
       <c r="C27" s="2">
         <f>C26/B26</f>
-        <v>10.833333333333334</v>
+        <v>4.056</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="4">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>